<commit_message>
Diesel Sounds, Alignment Stuff
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\GRFStuff\UK Finescale Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD60A6E-5C6E-4DD9-9420-2A7883238B7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC725AB7-76EB-488A-8347-589753AD309D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37095" yWindow="2250" windowWidth="19965" windowHeight="12675" activeTab="1" xr2:uid="{857BF7F3-4843-4495-BC2D-6D08C3451E58}"/>
+    <workbookView xWindow="37095" yWindow="2250" windowWidth="19965" windowHeight="12675" activeTab="2" xr2:uid="{857BF7F3-4843-4495-BC2D-6D08C3451E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Name Stuff" sheetId="4" r:id="rId1"/>
@@ -1976,111 +1976,6 @@
   </cellStyles>
   <dxfs count="35">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -2101,7 +1996,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+          <bgColor auto="1"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2127,7 +2022,7 @@
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
+          <bgColor indexed="65"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2590,6 +2485,111 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2604,38 +2604,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7575EDDE-3AAA-4483-ACE3-DCAE8EA3E8E7}" name="Table2" displayName="Table2" ref="A1:R101" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7575EDDE-3AAA-4483-ACE3-DCAE8EA3E8E7}" name="Table2" displayName="Table2" ref="A1:R101" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:R101" xr:uid="{36D57E6B-8B33-4ACF-A7F0-0856AF37967D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R101">
     <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{68CBBF4D-117B-46E6-B7A4-54509CD6E6FB}" name="ID" dataDxfId="32"/>
-    <tableColumn id="19" xr3:uid="{03AC1107-CE99-4984-A642-BF90BC17A239}" name="UKRS Name" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{BF20BF4A-0C5E-449A-ACE9-902DD6F25C69}" name="Weight" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{6F02F023-E63F-47BD-8453-9990FFD54AA5}" name="Speed" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{93D71C14-746F-4DF8-A137-B414A2B01F0B}" name="Power" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{4B59892B-E1F2-4F5C-BD85-8447BA247813}" name="TE" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{AC10C65A-66CC-4985-B3F7-B0FB085872AF}" name="TE Coeff" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{68CBBF4D-117B-46E6-B7A4-54509CD6E6FB}" name="ID" dataDxfId="17"/>
+    <tableColumn id="19" xr3:uid="{03AC1107-CE99-4984-A642-BF90BC17A239}" name="UKRS Name" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BF20BF4A-0C5E-449A-ACE9-902DD6F25C69}" name="Weight" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{6F02F023-E63F-47BD-8453-9990FFD54AA5}" name="Speed" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{93D71C14-746F-4DF8-A137-B414A2B01F0B}" name="Power" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{4B59892B-E1F2-4F5C-BD85-8447BA247813}" name="TE" dataDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{AC10C65A-66CC-4985-B3F7-B0FB085872AF}" name="TE Coeff" dataDxfId="11">
       <calculatedColumnFormula>F2/10/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7CCBBFAF-1597-42B4-A0E0-8848B36F3A85}" name="Cost" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{A935D94E-3872-4036-A743-42E97F0A5706}" name="Cost Factor" dataDxfId="24">
+    <tableColumn id="8" xr3:uid="{7CCBBFAF-1597-42B4-A0E0-8848B36F3A85}" name="Cost" dataDxfId="10"/>
+    <tableColumn id="9" xr3:uid="{A935D94E-3872-4036-A743-42E97F0A5706}" name="Cost Factor" dataDxfId="9">
       <calculatedColumnFormula>ROUNDDOWN(H2/1171,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{025F4854-003D-4C1D-86DE-3CE439FE9C7E}" name="RC Factor?" dataDxfId="23">
+    <tableColumn id="11" xr3:uid="{025F4854-003D-4C1D-86DE-3CE439FE9C7E}" name="RC Factor?" dataDxfId="8">
       <calculatedColumnFormula>Table2[[#This Row],[RunCost]]/(23400/255)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{5BCDCD29-35DE-42FD-B065-4D759BF7D38E}" name="New RC" dataDxfId="22">
+    <tableColumn id="14" xr3:uid="{5BCDCD29-35DE-42FD-B065-4D759BF7D38E}" name="New RC" dataDxfId="7">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(Table2[[#This Row],[Propulsion]],"S",Table2[[#This Row],[Cost Factor]]*(2090/255),"D",Table2[[#This Row],[Cost Factor]]*(1942/255),"E",Table2[[#This Row],[Cost Factor]]*(1792/255),"M",Table2[[#This Row],[Cost Factor]]*(1792/255),3,Table2[[#This Row],[Cost Factor]]*(1792/255))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{4EF97444-7DF2-4C1C-9399-2AF176D2421D}" name="RunCost" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{1BC97C8C-0238-41D7-8180-11A9FE8439B0}" name="Intro Year" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{5B6AB601-40E1-4161-8BD3-27417D3EF971}" name="Propulsion" dataDxfId="19"/>
-    <tableColumn id="15" xr3:uid="{3DD9EBC7-6915-4B09-94B8-EB93AD555BB9}" name="Length" dataDxfId="18"/>
-    <tableColumn id="16" xr3:uid="{6FAB79C9-0044-4515-B975-0FECD4FE0705}" name="Whistle" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{7544EFBE-4B04-489D-B161-77017965D88F}" name="Name" dataDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{AB5CB6B3-E247-433B-9AAE-1FAD1BCAC333}" name="FullName" dataDxfId="16">
+    <tableColumn id="10" xr3:uid="{4EF97444-7DF2-4C1C-9399-2AF176D2421D}" name="RunCost" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{1BC97C8C-0238-41D7-8180-11A9FE8439B0}" name="Intro Year" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{5B6AB601-40E1-4161-8BD3-27417D3EF971}" name="Propulsion" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{3DD9EBC7-6915-4B09-94B8-EB93AD555BB9}" name="Length" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{6FAB79C9-0044-4515-B975-0FECD4FE0705}" name="Whistle" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{7544EFBE-4B04-489D-B161-77017965D88F}" name="Name" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{AB5CB6B3-E247-433B-9AAE-1FAD1BCAC333}" name="FullName" dataDxfId="0">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[Name]]," - (",Table2[[#This Row],[UKRS Name]],")")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5288,7 +5288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8F614-8F67-461D-B4C9-7B9798EA7994}">
   <dimension ref="A1:AB101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N45" sqref="N45"/>
     </sheetView>
@@ -5403,14 +5403,14 @@
         <v>11</v>
       </c>
       <c r="G2" s="23">
-        <f>F2/10/C2</f>
+        <f t="shared" ref="G2:G33" si="0">F2/10/C2</f>
         <v>7.8571428571428584E-2</v>
       </c>
       <c r="H2" s="24">
         <v>7031</v>
       </c>
       <c r="I2" s="21">
-        <f>ROUNDDOWN(H2/1171,0)</f>
+        <f t="shared" ref="I2:I33" si="1">ROUNDDOWN(H2/1171,0)</f>
         <v>6</v>
       </c>
       <c r="J2" s="22">
@@ -5473,14 +5473,14 @@
         <v>43</v>
       </c>
       <c r="G3" s="23">
-        <f>F3/10/C3</f>
+        <f t="shared" si="0"/>
         <v>0.11621621621621621</v>
       </c>
       <c r="H3" s="24">
         <v>12890</v>
       </c>
       <c r="I3" s="21">
-        <f>ROUNDDOWN(H3/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J3" s="22">
@@ -5543,14 +5543,14 @@
         <v>21</v>
       </c>
       <c r="G4" s="23">
-        <f>F4/10/C4</f>
+        <f t="shared" si="0"/>
         <v>4.4680851063829789E-2</v>
       </c>
       <c r="H4" s="24">
         <v>16406</v>
       </c>
       <c r="I4" s="21">
-        <f>ROUNDDOWN(H4/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J4" s="22">
@@ -5613,14 +5613,14 @@
         <v>62</v>
       </c>
       <c r="G5" s="23">
-        <f>F5/10/C5</f>
+        <f t="shared" si="0"/>
         <v>0.14761904761904762</v>
       </c>
       <c r="H5" s="24">
         <v>15234</v>
       </c>
       <c r="I5" s="21">
-        <f>ROUNDDOWN(H5/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="J5" s="22">
@@ -5683,14 +5683,14 @@
         <v>79</v>
       </c>
       <c r="G6" s="23">
-        <f>F6/10/C6</f>
+        <f t="shared" si="0"/>
         <v>0.22571428571428573</v>
       </c>
       <c r="H6" s="24">
         <v>8203</v>
       </c>
       <c r="I6" s="21">
-        <f>ROUNDDOWN(H6/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="J6" s="22">
@@ -5753,14 +5753,14 @@
         <v>39</v>
       </c>
       <c r="G7" s="23">
-        <f>F7/10/C7</f>
+        <f t="shared" si="0"/>
         <v>0.13928571428571429</v>
       </c>
       <c r="H7" s="24">
         <v>9375</v>
       </c>
       <c r="I7" s="21">
-        <f>ROUNDDOWN(H7/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="J7" s="22">
@@ -5823,14 +5823,14 @@
         <v>104</v>
       </c>
       <c r="G8" s="23">
-        <f>F8/10/C8</f>
+        <f t="shared" si="0"/>
         <v>0.21666666666666667</v>
       </c>
       <c r="H8" s="24">
         <v>12890</v>
       </c>
       <c r="I8" s="21">
-        <f>ROUNDDOWN(H8/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J8" s="22">
@@ -5893,14 +5893,14 @@
         <v>55</v>
       </c>
       <c r="G9" s="23">
-        <f>F9/10/C9</f>
+        <f t="shared" si="0"/>
         <v>0.15277777777777779</v>
       </c>
       <c r="H9" s="24">
         <v>12890</v>
       </c>
       <c r="I9" s="21">
-        <f>ROUNDDOWN(H9/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J9" s="22">
@@ -5963,14 +5963,14 @@
         <v>55</v>
       </c>
       <c r="G10" s="23">
-        <f>F10/10/C10</f>
+        <f t="shared" si="0"/>
         <v>0.15277777777777779</v>
       </c>
       <c r="H10" s="24">
         <v>12890</v>
       </c>
       <c r="I10" s="21">
-        <f>ROUNDDOWN(H10/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="J10" s="22">
@@ -6033,14 +6033,14 @@
         <v>57</v>
       </c>
       <c r="G11" s="23">
-        <f>F11/10/C11</f>
+        <f t="shared" si="0"/>
         <v>0.114</v>
       </c>
       <c r="H11" s="24">
         <v>17578</v>
       </c>
       <c r="I11" s="21">
-        <f>ROUNDDOWN(H11/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J11" s="22">
@@ -6103,14 +6103,14 @@
         <v>88</v>
       </c>
       <c r="G12" s="23">
-        <f>F12/10/C12</f>
+        <f t="shared" si="0"/>
         <v>0.17600000000000002</v>
       </c>
       <c r="H12" s="24">
         <v>17578</v>
       </c>
       <c r="I12" s="21">
-        <f>ROUNDDOWN(H12/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J12" s="22">
@@ -6173,14 +6173,14 @@
         <v>88</v>
       </c>
       <c r="G13" s="23">
-        <f>F13/10/C13</f>
+        <f t="shared" si="0"/>
         <v>0.17600000000000002</v>
       </c>
       <c r="H13" s="24">
         <v>17578</v>
       </c>
       <c r="I13" s="21">
-        <f>ROUNDDOWN(H13/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J13" s="22">
@@ -6243,14 +6243,14 @@
         <v>78</v>
       </c>
       <c r="G14" s="23">
-        <f>F14/10/C14</f>
+        <f t="shared" si="0"/>
         <v>0.12580645161290321</v>
       </c>
       <c r="H14" s="24">
         <v>18750</v>
       </c>
       <c r="I14" s="21">
-        <f>ROUNDDOWN(H14/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J14" s="22">
@@ -6313,14 +6313,14 @@
         <v>93</v>
       </c>
       <c r="G15" s="23">
-        <f>F15/10/C15</f>
+        <f t="shared" si="0"/>
         <v>0.16315789473684211</v>
       </c>
       <c r="H15" s="24">
         <v>19921</v>
       </c>
       <c r="I15" s="21">
-        <f>ROUNDDOWN(H15/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J15" s="22">
@@ -6383,14 +6383,14 @@
         <v>40</v>
       </c>
       <c r="G16" s="23">
-        <f>F16/10/C16</f>
+        <f t="shared" si="0"/>
         <v>8.6956521739130432E-2</v>
       </c>
       <c r="H16" s="24">
         <v>16406</v>
       </c>
       <c r="I16" s="21">
-        <f>ROUNDDOWN(H16/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="J16" s="22">
@@ -6453,14 +6453,14 @@
         <v>45</v>
       </c>
       <c r="G17" s="23">
-        <f>F17/10/C17</f>
+        <f t="shared" si="0"/>
         <v>8.0357142857142863E-2</v>
       </c>
       <c r="H17" s="24">
         <v>19921</v>
       </c>
       <c r="I17" s="21">
-        <f>ROUNDDOWN(H17/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J17" s="22">
@@ -6523,14 +6523,14 @@
         <v>78</v>
       </c>
       <c r="G18" s="23">
-        <f>F18/10/C18</f>
+        <f t="shared" si="0"/>
         <v>0.10985915492957746</v>
       </c>
       <c r="H18" s="24">
         <v>24609</v>
       </c>
       <c r="I18" s="21">
-        <f>ROUNDDOWN(H18/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="J18" s="22">
@@ -6594,14 +6594,14 @@
         <v>70</v>
       </c>
       <c r="G19" s="23">
-        <f>F19/10/C19</f>
+        <f t="shared" si="0"/>
         <v>6.4814814814814811E-2</v>
       </c>
       <c r="H19" s="24">
         <v>31640</v>
       </c>
       <c r="I19" s="21">
-        <f>ROUNDDOWN(H19/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="J19" s="22">
@@ -6664,14 +6664,14 @@
         <v>97</v>
       </c>
       <c r="G20" s="23">
-        <f>F20/10/C20</f>
+        <f t="shared" si="0"/>
         <v>9.509803921568627E-2</v>
       </c>
       <c r="H20" s="24">
         <v>30468</v>
       </c>
       <c r="I20" s="21">
-        <f>ROUNDDOWN(H20/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J20" s="22">
@@ -6734,14 +6734,14 @@
         <v>110</v>
       </c>
       <c r="G21" s="23">
-        <f>F21/10/C21</f>
+        <f t="shared" si="0"/>
         <v>0.12222222222222222</v>
       </c>
       <c r="H21" s="24">
         <v>26953</v>
       </c>
       <c r="I21" s="21">
-        <f>ROUNDDOWN(H21/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="J21" s="22">
@@ -6804,14 +6804,14 @@
         <v>112</v>
       </c>
       <c r="G22" s="23">
-        <f>F22/10/C22</f>
+        <f t="shared" si="0"/>
         <v>0.10666666666666666</v>
       </c>
       <c r="H22" s="24">
         <v>30468</v>
       </c>
       <c r="I22" s="21">
-        <f>ROUNDDOWN(H22/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J22" s="22">
@@ -6874,14 +6874,14 @@
         <v>122</v>
       </c>
       <c r="G23" s="23">
-        <f>F23/10/C23</f>
+        <f t="shared" si="0"/>
         <v>0.12978723404255318</v>
       </c>
       <c r="H23" s="24">
         <v>28125</v>
       </c>
       <c r="I23" s="21">
-        <f>ROUNDDOWN(H23/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="J23" s="22">
@@ -6944,14 +6944,14 @@
         <v>190</v>
       </c>
       <c r="G24" s="23">
-        <f>F24/10/C24</f>
+        <f t="shared" si="0"/>
         <v>0.17924528301886791</v>
       </c>
       <c r="H24" s="24">
         <v>31640</v>
       </c>
       <c r="I24" s="21">
-        <f>ROUNDDOWN(H24/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="J24" s="22">
@@ -7015,14 +7015,14 @@
         <v>105</v>
       </c>
       <c r="G25" s="23">
-        <f>F25/10/C25</f>
+        <f t="shared" si="0"/>
         <v>7.6086956521739135E-2</v>
       </c>
       <c r="H25" s="24">
         <v>41015</v>
       </c>
       <c r="I25" s="21">
-        <f>ROUNDDOWN(H25/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="J25" s="22">
@@ -7086,14 +7086,14 @@
         <v>99</v>
       </c>
       <c r="G26" s="23">
-        <f>F26/10/C26</f>
+        <f t="shared" si="0"/>
         <v>0.20204081632653062</v>
       </c>
       <c r="H26" s="24">
         <v>17578</v>
       </c>
       <c r="I26" s="21">
-        <f>ROUNDDOWN(H26/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="J26" s="22">
@@ -7156,14 +7156,14 @@
         <v>98</v>
       </c>
       <c r="G27" s="23">
-        <f>F27/10/C27</f>
+        <f t="shared" si="0"/>
         <v>0.17818181818181819</v>
       </c>
       <c r="H27" s="24">
         <v>19921</v>
       </c>
       <c r="I27" s="21">
-        <f>ROUNDDOWN(H27/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="J27" s="22">
@@ -7226,14 +7226,14 @@
         <v>75</v>
       </c>
       <c r="G28" s="23">
-        <f>F28/10/C28</f>
+        <f t="shared" si="0"/>
         <v>0.1171875</v>
       </c>
       <c r="H28" s="24">
         <v>22265</v>
       </c>
       <c r="I28" s="21">
-        <f>ROUNDDOWN(H28/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="J28" s="22">
@@ -7297,14 +7297,14 @@
         <v>107</v>
       </c>
       <c r="G29" s="23">
-        <f>F29/10/C29</f>
+        <f t="shared" si="0"/>
         <v>0.12159090909090908</v>
       </c>
       <c r="H29" s="24">
         <v>30468</v>
       </c>
       <c r="I29" s="21">
-        <f>ROUNDDOWN(H29/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="J29" s="22">
@@ -7367,14 +7367,14 @@
         <v>130</v>
       </c>
       <c r="G30" s="23">
-        <f>F30/10/C30</f>
+        <f t="shared" si="0"/>
         <v>0.14444444444444443</v>
       </c>
       <c r="H30" s="24">
         <v>23437</v>
       </c>
       <c r="I30" s="21">
-        <f>ROUNDDOWN(H30/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="J30" s="22">
@@ -7437,14 +7437,14 @@
         <v>95</v>
       </c>
       <c r="G31" s="23">
-        <f>F31/10/C31</f>
+        <f t="shared" si="0"/>
         <v>7.9831932773109238E-2</v>
       </c>
       <c r="H31" s="24">
         <v>35156</v>
       </c>
       <c r="I31" s="21">
-        <f>ROUNDDOWN(H31/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="J31" s="22">
@@ -7507,14 +7507,14 @@
         <v>110</v>
       </c>
       <c r="G32" s="23">
-        <f>F32/10/C32</f>
+        <f t="shared" si="0"/>
         <v>8.0291970802919707E-2</v>
       </c>
       <c r="H32" s="24">
         <v>39843</v>
       </c>
       <c r="I32" s="21">
-        <f>ROUNDDOWN(H32/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="J32" s="22">
@@ -7577,14 +7577,14 @@
         <v>202</v>
       </c>
       <c r="G33" s="23">
-        <f>F33/10/C33</f>
+        <f t="shared" si="0"/>
         <v>0.1337748344370861</v>
       </c>
       <c r="H33" s="24">
         <v>44531</v>
       </c>
       <c r="I33" s="21">
-        <f>ROUNDDOWN(H33/1171,0)</f>
+        <f t="shared" si="1"/>
         <v>38</v>
       </c>
       <c r="J33" s="22">
@@ -7647,14 +7647,14 @@
         <v>142</v>
       </c>
       <c r="G34" s="23">
-        <f>F34/10/C34</f>
+        <f t="shared" ref="G34:G65" si="2">F34/10/C34</f>
         <v>0.11093749999999999</v>
       </c>
       <c r="H34" s="24">
         <v>37500</v>
       </c>
       <c r="I34" s="21">
-        <f>ROUNDDOWN(H34/1171,0)</f>
+        <f t="shared" ref="I34:I65" si="3">ROUNDDOWN(H34/1171,0)</f>
         <v>32</v>
       </c>
       <c r="J34" s="22">
@@ -7717,14 +7717,14 @@
         <v>115</v>
       </c>
       <c r="G35" s="23">
-        <f>F35/10/C35</f>
+        <f t="shared" si="2"/>
         <v>9.1269841269841265E-2</v>
       </c>
       <c r="H35" s="24">
         <v>37500</v>
       </c>
       <c r="I35" s="21">
-        <f>ROUNDDOWN(H35/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>32</v>
       </c>
       <c r="J35" s="22">
@@ -7787,14 +7787,14 @@
         <v>148</v>
       </c>
       <c r="G36" s="23">
-        <f>F36/10/C36</f>
+        <f t="shared" si="2"/>
         <v>0.10277777777777779</v>
       </c>
       <c r="H36" s="24">
         <v>42187</v>
       </c>
       <c r="I36" s="21">
-        <f>ROUNDDOWN(H36/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="J36" s="22">
@@ -7857,14 +7857,14 @@
         <v>132</v>
       </c>
       <c r="G37" s="23">
-        <f>F37/10/C37</f>
+        <f t="shared" si="2"/>
         <v>8.7417218543046349E-2</v>
       </c>
       <c r="H37" s="24">
         <v>44531</v>
       </c>
       <c r="I37" s="21">
-        <f>ROUNDDOWN(H37/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="J37" s="22">
@@ -7928,14 +7928,14 @@
         <v>158</v>
       </c>
       <c r="G38" s="23">
-        <f>F38/10/C38</f>
+        <f t="shared" si="2"/>
         <v>9.5180722891566275E-2</v>
       </c>
       <c r="H38" s="24">
         <v>49218</v>
       </c>
       <c r="I38" s="21">
-        <f>ROUNDDOWN(H38/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="J38" s="22">
@@ -7999,14 +7999,14 @@
         <v>182</v>
       </c>
       <c r="G39" s="23">
-        <f>F39/10/C39</f>
+        <f t="shared" si="2"/>
         <v>0.11097560975609756</v>
       </c>
       <c r="H39" s="24">
         <v>48046</v>
       </c>
       <c r="I39" s="21">
-        <f>ROUNDDOWN(H39/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>41</v>
       </c>
       <c r="J39" s="22">
@@ -8069,14 +8069,14 @@
         <v>165</v>
       </c>
       <c r="G40" s="23">
-        <f>F40/10/C40</f>
+        <f t="shared" si="2"/>
         <v>0.11458333333333333</v>
       </c>
       <c r="H40" s="24">
         <v>42187</v>
       </c>
       <c r="I40" s="21">
-        <f>ROUNDDOWN(H40/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="J40" s="22">
@@ -8139,14 +8139,14 @@
         <v>136</v>
       </c>
       <c r="G41" s="23">
-        <f>F41/10/C41</f>
+        <f t="shared" si="2"/>
         <v>0.10303030303030303</v>
       </c>
       <c r="H41" s="24">
         <v>38671</v>
       </c>
       <c r="I41" s="21">
-        <f>ROUNDDOWN(H41/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="J41" s="22">
@@ -8209,14 +8209,14 @@
         <v>204</v>
       </c>
       <c r="G42" s="23">
-        <f>F42/10/C42</f>
+        <f t="shared" si="2"/>
         <v>0.15692307692307692</v>
       </c>
       <c r="H42" s="24">
         <v>45703</v>
       </c>
       <c r="I42" s="21">
-        <f>ROUNDDOWN(H42/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="J42" s="22">
@@ -8280,14 +8280,14 @@
         <v>143</v>
       </c>
       <c r="G43" s="23">
-        <f>F43/10/C43</f>
+        <f t="shared" si="2"/>
         <v>9.9305555555555564E-2</v>
       </c>
       <c r="H43" s="24">
         <v>42187</v>
       </c>
       <c r="I43" s="21">
-        <f>ROUNDDOWN(H43/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="J43" s="22">
@@ -8351,14 +8351,14 @@
         <v>178</v>
       </c>
       <c r="G44" s="23">
-        <f>F44/10/C44</f>
+        <f t="shared" si="2"/>
         <v>0.12624113475177307</v>
       </c>
       <c r="H44" s="24">
         <v>41015</v>
       </c>
       <c r="I44" s="21">
-        <f>ROUNDDOWN(H44/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="J44" s="22">
@@ -8423,14 +8423,14 @@
         <v>169</v>
       </c>
       <c r="G45" s="23">
-        <f>F45/10/C45</f>
+        <f t="shared" si="2"/>
         <v>0.13739837398373983</v>
       </c>
       <c r="H45" s="24">
         <v>72656</v>
       </c>
       <c r="I45" s="21">
-        <f>ROUNDDOWN(H45/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>62</v>
       </c>
       <c r="J45" s="22">
@@ -8490,14 +8490,14 @@
         <v>155</v>
       </c>
       <c r="G46" s="29">
-        <f>F46/10/C46</f>
+        <f t="shared" si="2"/>
         <v>0.31</v>
       </c>
       <c r="H46" s="30">
         <v>8203</v>
       </c>
       <c r="I46" s="27">
-        <f>ROUNDDOWN(H46/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="J46" s="28">
@@ -8561,14 +8561,14 @@
         <v>135</v>
       </c>
       <c r="G47" s="29">
-        <f>F47/10/C47</f>
+        <f t="shared" si="2"/>
         <v>0.28125</v>
       </c>
       <c r="H47" s="30">
         <v>9375</v>
       </c>
       <c r="I47" s="27">
-        <f>ROUNDDOWN(H47/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="J47" s="28">
@@ -8632,14 +8632,14 @@
         <v>187</v>
       </c>
       <c r="G48" s="29">
-        <f>F48/10/C48</f>
+        <f t="shared" si="2"/>
         <v>0.25616438356164384</v>
       </c>
       <c r="H48" s="30">
         <v>17578</v>
       </c>
       <c r="I48" s="27">
-        <f>ROUNDDOWN(H48/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="J48" s="28">
@@ -8703,14 +8703,14 @@
         <v>176</v>
       </c>
       <c r="G49" s="29">
-        <f>F49/10/C49</f>
+        <f t="shared" si="2"/>
         <v>0.25507246376811599</v>
       </c>
       <c r="H49" s="30">
         <v>12890</v>
       </c>
       <c r="I49" s="27">
-        <f>ROUNDDOWN(H49/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="J49" s="28">
@@ -8774,14 +8774,14 @@
         <v>187</v>
       </c>
       <c r="G50" s="29">
-        <f>F50/10/C50</f>
+        <f t="shared" si="2"/>
         <v>0.25972222222222219</v>
       </c>
       <c r="H50" s="30">
         <v>21093</v>
       </c>
       <c r="I50" s="27">
-        <f>ROUNDDOWN(H50/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="J50" s="28">
@@ -8845,14 +8845,14 @@
         <v>192</v>
       </c>
       <c r="G51" s="29">
-        <f>F51/10/C51</f>
+        <f t="shared" si="2"/>
         <v>0.25945945945945947</v>
       </c>
       <c r="H51" s="30">
         <v>18750</v>
       </c>
       <c r="I51" s="27">
-        <f>ROUNDDOWN(H51/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="J51" s="28">
@@ -8916,14 +8916,14 @@
         <v>184</v>
       </c>
       <c r="G52" s="29">
-        <f>F52/10/C52</f>
+        <f t="shared" si="2"/>
         <v>0.14153846153846153</v>
       </c>
       <c r="H52" s="30">
         <v>42187</v>
       </c>
       <c r="I52" s="27">
-        <f>ROUNDDOWN(H52/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>36</v>
       </c>
       <c r="J52" s="28">
@@ -8987,14 +8987,14 @@
         <v>253</v>
       </c>
       <c r="G53" s="29">
-        <f>F53/10/C53</f>
+        <f t="shared" si="2"/>
         <v>0.23644859813084113</v>
       </c>
       <c r="H53" s="30">
         <v>32812</v>
       </c>
       <c r="I53" s="27">
-        <f>ROUNDDOWN(H53/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>28</v>
       </c>
       <c r="J53" s="28">
@@ -9058,14 +9058,14 @@
         <v>212</v>
       </c>
       <c r="G54" s="29">
-        <f>F54/10/C54</f>
+        <f t="shared" si="2"/>
         <v>0.27179487179487177</v>
       </c>
       <c r="H54" s="30">
         <v>35156</v>
       </c>
       <c r="I54" s="27">
-        <f>ROUNDDOWN(H54/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
       <c r="J54" s="28">
@@ -9129,14 +9129,14 @@
         <v>297</v>
       </c>
       <c r="G55" s="29">
-        <f>F55/10/C55</f>
+        <f t="shared" si="2"/>
         <v>0.27499999999999997</v>
       </c>
       <c r="H55" s="30">
         <v>59765</v>
       </c>
       <c r="I55" s="27">
-        <f>ROUNDDOWN(H55/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
       <c r="J55" s="28">
@@ -9200,14 +9200,14 @@
         <v>248</v>
       </c>
       <c r="G56" s="29">
-        <f>F56/10/C56</f>
+        <f t="shared" si="2"/>
         <v>0.1837037037037037</v>
       </c>
       <c r="H56" s="30">
         <v>53906</v>
       </c>
       <c r="I56" s="27">
-        <f>ROUNDDOWN(H56/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>46</v>
       </c>
       <c r="J56" s="28">
@@ -9271,14 +9271,14 @@
         <v>266</v>
       </c>
       <c r="G57" s="29">
-        <f>F57/10/C57</f>
+        <f t="shared" si="2"/>
         <v>0.22166666666666668</v>
       </c>
       <c r="H57" s="30">
         <v>45703</v>
       </c>
       <c r="I57" s="27">
-        <f>ROUNDDOWN(H57/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
       <c r="J57" s="28">
@@ -9342,14 +9342,14 @@
         <v>220</v>
       </c>
       <c r="G58" s="29">
-        <f>F58/10/C58</f>
+        <f t="shared" si="2"/>
         <v>0.21782178217821782</v>
       </c>
       <c r="H58" s="30">
         <v>78515</v>
       </c>
       <c r="I58" s="27">
-        <f>ROUNDDOWN(H58/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>67</v>
       </c>
       <c r="J58" s="28">
@@ -9413,14 +9413,14 @@
         <v>271</v>
       </c>
       <c r="G59" s="29">
-        <f>F59/10/C59</f>
+        <f t="shared" si="2"/>
         <v>0.21007751937984498</v>
       </c>
       <c r="H59" s="30">
         <v>50390</v>
       </c>
       <c r="I59" s="27">
-        <f>ROUNDDOWN(H59/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="J59" s="28">
@@ -9484,14 +9484,14 @@
         <v>474</v>
       </c>
       <c r="G60" s="29">
-        <f>F60/10/C60</f>
+        <f t="shared" si="2"/>
         <v>0.36744186046511629</v>
       </c>
       <c r="H60" s="30">
         <v>46875</v>
       </c>
       <c r="I60" s="27">
-        <f>ROUNDDOWN(H60/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>40</v>
       </c>
       <c r="J60" s="28">
@@ -9555,14 +9555,14 @@
         <v>411</v>
       </c>
       <c r="G61" s="29">
-        <f>F61/10/C61</f>
+        <f t="shared" si="2"/>
         <v>0.32109375000000001</v>
       </c>
       <c r="H61" s="30">
         <v>49218</v>
       </c>
       <c r="I61" s="27">
-        <f>ROUNDDOWN(H61/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>42</v>
       </c>
       <c r="J61" s="28">
@@ -9626,14 +9626,14 @@
         <v>144</v>
       </c>
       <c r="G62" s="29">
-        <f>F62/10/C62</f>
+        <f t="shared" si="2"/>
         <v>0.16363636363636364</v>
       </c>
       <c r="H62" s="30">
         <v>43359</v>
       </c>
       <c r="I62" s="27">
-        <f>ROUNDDOWN(H62/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="J62" s="28">
@@ -9697,14 +9697,14 @@
         <v>533</v>
       </c>
       <c r="G63" s="29">
-        <f>F63/10/C63</f>
+        <f t="shared" si="2"/>
         <v>0.41317829457364341</v>
       </c>
       <c r="H63" s="30">
         <v>56250</v>
       </c>
       <c r="I63" s="27">
-        <f>ROUNDDOWN(H63/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="J63" s="28">
@@ -9768,14 +9768,14 @@
         <v>176</v>
       </c>
       <c r="G64" s="20">
-        <f>F64/10/C64</f>
+        <f t="shared" si="2"/>
         <v>0.22857142857142859</v>
       </c>
       <c r="H64" s="18">
         <v>25781</v>
       </c>
       <c r="I64" s="13">
-        <f>ROUNDDOWN(H64/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="J64" s="15">
@@ -9840,14 +9840,14 @@
         <v>177</v>
       </c>
       <c r="G65" s="20">
-        <f>F65/10/C65</f>
+        <f t="shared" si="2"/>
         <v>0.17524752475247524</v>
       </c>
       <c r="H65" s="18">
         <v>43359</v>
       </c>
       <c r="I65" s="13">
-        <f>ROUNDDOWN(H65/1171,0)</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="J65" s="15">
@@ -9912,14 +9912,14 @@
         <v>194</v>
       </c>
       <c r="G66" s="20">
-        <f>F66/10/C66</f>
+        <f t="shared" ref="G66:G97" si="4">F66/10/C66</f>
         <v>0.24871794871794869</v>
       </c>
       <c r="H66" s="18">
         <v>35156</v>
       </c>
       <c r="I66" s="13">
-        <f>ROUNDDOWN(H66/1171,0)</f>
+        <f t="shared" ref="I66:I97" si="5">ROUNDDOWN(H66/1171,0)</f>
         <v>30</v>
       </c>
       <c r="J66" s="15">
@@ -9984,14 +9984,14 @@
         <v>118</v>
       </c>
       <c r="G67" s="20">
-        <f>F67/10/C67</f>
+        <f t="shared" si="4"/>
         <v>0.15945945945945947</v>
       </c>
       <c r="H67" s="18">
         <v>31640</v>
       </c>
       <c r="I67" s="13">
-        <f>ROUNDDOWN(H67/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="J67" s="15">
@@ -10056,14 +10056,14 @@
         <v>117</v>
       </c>
       <c r="G68" s="20">
-        <f>F68/10/C68</f>
+        <f t="shared" si="4"/>
         <v>0.10636363636363635</v>
       </c>
       <c r="H68" s="18">
         <v>77343</v>
       </c>
       <c r="I68" s="13">
-        <f>ROUNDDOWN(H68/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>66</v>
       </c>
       <c r="J68" s="15">
@@ -10128,14 +10128,14 @@
         <v>199</v>
       </c>
       <c r="G69" s="20">
-        <f>F69/10/C69</f>
+        <f t="shared" si="4"/>
         <v>0.22873563218390802</v>
       </c>
       <c r="H69" s="18">
         <v>35156</v>
       </c>
       <c r="I69" s="13">
-        <f>ROUNDDOWN(H69/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="J69" s="15">
@@ -10200,14 +10200,14 @@
         <v>199</v>
       </c>
       <c r="G70" s="20">
-        <f>F70/10/C70</f>
+        <f t="shared" si="4"/>
         <v>0.19134615384615383</v>
       </c>
       <c r="H70" s="18">
         <v>76171</v>
       </c>
       <c r="I70" s="13">
-        <f>ROUNDDOWN(H70/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>65</v>
       </c>
       <c r="J70" s="15">
@@ -10272,14 +10272,14 @@
         <v>220</v>
       </c>
       <c r="G71" s="20">
-        <f>F71/10/C71</f>
+        <f t="shared" si="4"/>
         <v>0.27848101265822783</v>
       </c>
       <c r="H71" s="18">
         <v>37500</v>
       </c>
       <c r="I71" s="13">
-        <f>ROUNDDOWN(H71/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>32</v>
       </c>
       <c r="J71" s="15">
@@ -10344,14 +10344,14 @@
         <v>257</v>
       </c>
       <c r="G72" s="20">
-        <f>F72/10/C72</f>
+        <f t="shared" si="4"/>
         <v>0.31728395061728393</v>
       </c>
       <c r="H72" s="18">
         <v>42187</v>
       </c>
       <c r="I72" s="13">
-        <f>ROUNDDOWN(H72/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>36</v>
       </c>
       <c r="J72" s="15">
@@ -10416,14 +10416,14 @@
         <v>204</v>
       </c>
       <c r="G73" s="20">
-        <f>F73/10/C73</f>
+        <f t="shared" si="4"/>
         <v>0.19428571428571428</v>
       </c>
       <c r="H73" s="18">
         <v>107812</v>
       </c>
       <c r="I73" s="13">
-        <f>ROUNDDOWN(H73/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>92</v>
       </c>
       <c r="J73" s="15">
@@ -10488,14 +10488,14 @@
         <v>257</v>
       </c>
       <c r="G74" s="20">
-        <f>F74/10/C74</f>
+        <f t="shared" si="4"/>
         <v>0.30595238095238092</v>
       </c>
       <c r="H74" s="18">
         <v>73828</v>
       </c>
       <c r="I74" s="13">
-        <f>ROUNDDOWN(H74/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="J74" s="15">
@@ -10560,14 +10560,14 @@
         <v>356</v>
       </c>
       <c r="G75" s="20">
-        <f>F75/10/C75</f>
+        <f t="shared" si="4"/>
         <v>0.28253968253968254</v>
       </c>
       <c r="H75" s="18">
         <v>132421</v>
       </c>
       <c r="I75" s="13">
-        <f>ROUNDDOWN(H75/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>113</v>
       </c>
       <c r="J75" s="15">
@@ -10632,14 +10632,14 @@
         <v>218</v>
       </c>
       <c r="G76" s="20">
-        <f>F76/10/C76</f>
+        <f t="shared" si="4"/>
         <v>0.32537313432835824</v>
       </c>
       <c r="H76" s="18">
         <v>18750</v>
       </c>
       <c r="I76" s="13">
-        <f>ROUNDDOWN(H76/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
       <c r="J76" s="15">
@@ -10704,14 +10704,14 @@
         <v>380</v>
       </c>
       <c r="G77" s="20">
-        <f>F77/10/C77</f>
+        <f t="shared" si="4"/>
         <v>0.27142857142857141</v>
       </c>
       <c r="H77" s="18">
         <v>131250</v>
       </c>
       <c r="I77" s="13">
-        <f>ROUNDDOWN(H77/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>112</v>
       </c>
       <c r="J77" s="15">
@@ -10776,14 +10776,14 @@
         <v>222</v>
       </c>
       <c r="G78" s="20">
-        <f>F78/10/C78</f>
+        <f t="shared" si="4"/>
         <v>0.19473684210526315</v>
       </c>
       <c r="H78" s="18">
         <v>92578</v>
       </c>
       <c r="I78" s="13">
-        <f>ROUNDDOWN(H78/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="J78" s="15">
@@ -10848,14 +10848,14 @@
         <v>348</v>
       </c>
       <c r="G79" s="20">
-        <f>F79/10/C79</f>
+        <f t="shared" si="4"/>
         <v>0.25217391304347825</v>
       </c>
       <c r="H79" s="18">
         <v>298828</v>
       </c>
       <c r="I79" s="13">
-        <f>ROUNDDOWN(H79/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>255</v>
       </c>
       <c r="J79" s="15">
@@ -10920,14 +10920,14 @@
         <v>19</v>
       </c>
       <c r="G80" s="20">
-        <f>F80/10/C80</f>
+        <f t="shared" si="4"/>
         <v>5.2777777777777778E-2</v>
       </c>
       <c r="H80" s="18">
         <v>12890</v>
       </c>
       <c r="I80" s="13">
-        <f>ROUNDDOWN(H80/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="J80" s="15">
@@ -10992,14 +10992,14 @@
         <v>19</v>
       </c>
       <c r="G81" s="20">
-        <f>F81/10/C81</f>
+        <f t="shared" si="4"/>
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="H81" s="18">
         <v>3515</v>
       </c>
       <c r="I81" s="13">
-        <f>ROUNDDOWN(H81/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J81" s="15">
@@ -11064,14 +11064,14 @@
         <v>34</v>
       </c>
       <c r="G82" s="20">
-        <f>F82/10/C82</f>
+        <f t="shared" si="4"/>
         <v>0.11724137931034483</v>
       </c>
       <c r="H82" s="18">
         <v>7031</v>
       </c>
       <c r="I82" s="13">
-        <f>ROUNDDOWN(H82/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="J82" s="15">
@@ -11136,14 +11136,14 @@
         <v>80</v>
       </c>
       <c r="G83" s="20">
-        <f>F83/10/C83</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
       <c r="H83" s="18">
         <v>22265</v>
       </c>
       <c r="I83" s="13">
-        <f>ROUNDDOWN(H83/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="J83" s="15">
@@ -11208,14 +11208,14 @@
         <v>90</v>
       </c>
       <c r="G84" s="20">
-        <f>F84/10/C84</f>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
       <c r="H84" s="18">
         <v>24609</v>
       </c>
       <c r="I84" s="13">
-        <f>ROUNDDOWN(H84/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J84" s="15">
@@ -11280,14 +11280,14 @@
         <v>98</v>
       </c>
       <c r="G85" s="20">
-        <f>F85/10/C85</f>
+        <f t="shared" si="4"/>
         <v>0.12894736842105264</v>
       </c>
       <c r="H85" s="18">
         <v>26953</v>
       </c>
       <c r="I85" s="13">
-        <f>ROUNDDOWN(H85/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="J85" s="15">
@@ -11352,14 +11352,14 @@
         <v>141</v>
       </c>
       <c r="G86" s="20">
-        <f>F86/10/C86</f>
+        <f t="shared" si="4"/>
         <v>0.15666666666666668</v>
       </c>
       <c r="H86" s="18">
         <v>39843</v>
       </c>
       <c r="I86" s="13">
-        <f>ROUNDDOWN(H86/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="J86" s="15">
@@ -11424,14 +11424,14 @@
         <v>158</v>
       </c>
       <c r="G87" s="20">
-        <f>F87/10/C87</f>
+        <f t="shared" si="4"/>
         <v>0.18372093023255814</v>
       </c>
       <c r="H87" s="18">
         <v>60937</v>
       </c>
       <c r="I87" s="13">
-        <f>ROUNDDOWN(H87/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="J87" s="15">
@@ -11496,14 +11496,14 @@
         <v>160</v>
       </c>
       <c r="G88" s="20">
-        <f>F88/10/C88</f>
+        <f t="shared" si="4"/>
         <v>0.11428571428571428</v>
       </c>
       <c r="H88" s="18">
         <v>73828</v>
       </c>
       <c r="I88" s="13">
-        <f>ROUNDDOWN(H88/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>63</v>
       </c>
       <c r="J88" s="15">
@@ -11568,14 +11568,14 @@
         <v>83</v>
       </c>
       <c r="G89" s="20">
-        <f>F89/10/C89</f>
+        <f t="shared" si="4"/>
         <v>0.12205882352941178</v>
       </c>
       <c r="H89" s="18">
         <v>29296</v>
       </c>
       <c r="I89" s="13">
-        <f>ROUNDDOWN(H89/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="J89" s="15">
@@ -11640,14 +11640,14 @@
         <v>68</v>
       </c>
       <c r="G90" s="20">
-        <f>F90/10/C90</f>
+        <f t="shared" si="4"/>
         <v>8.9473684210526316E-2</v>
       </c>
       <c r="H90" s="18">
         <v>26953</v>
       </c>
       <c r="I90" s="13">
-        <f>ROUNDDOWN(H90/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="J90" s="15">
@@ -11712,14 +11712,14 @@
         <v>135</v>
       </c>
       <c r="G91" s="20">
-        <f>F91/10/C91</f>
+        <f t="shared" si="4"/>
         <v>0.1875</v>
       </c>
       <c r="H91" s="18">
         <v>24609</v>
       </c>
       <c r="I91" s="13">
-        <f>ROUNDDOWN(H91/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J91" s="15">
@@ -11784,14 +11784,14 @@
         <v>140</v>
       </c>
       <c r="G92" s="20">
-        <f>F92/10/C92</f>
+        <f t="shared" si="4"/>
         <v>0.17948717948717949</v>
       </c>
       <c r="H92" s="18">
         <v>31640</v>
       </c>
       <c r="I92" s="13">
-        <f>ROUNDDOWN(H92/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>27</v>
       </c>
       <c r="J92" s="15">
@@ -11856,14 +11856,14 @@
         <v>130</v>
       </c>
       <c r="G93" s="20">
-        <f>F93/10/C93</f>
+        <f t="shared" si="4"/>
         <v>0.14130434782608695</v>
       </c>
       <c r="H93" s="18">
         <v>26953</v>
       </c>
       <c r="I93" s="13">
-        <f>ROUNDDOWN(H93/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>23</v>
       </c>
       <c r="J93" s="15">
@@ -11928,14 +11928,14 @@
         <v>126</v>
       </c>
       <c r="G94" s="20">
-        <f>F94/10/C94</f>
+        <f t="shared" si="4"/>
         <v>0.17499999999999999</v>
       </c>
       <c r="H94" s="18">
         <v>21093</v>
       </c>
       <c r="I94" s="13">
-        <f>ROUNDDOWN(H94/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="J94" s="15">
@@ -12000,14 +12000,14 @@
         <v>147</v>
       </c>
       <c r="G95" s="20">
-        <f>F95/10/C95</f>
+        <f t="shared" si="4"/>
         <v>0.17926829268292682</v>
       </c>
       <c r="H95" s="18">
         <v>29296</v>
       </c>
       <c r="I95" s="13">
-        <f>ROUNDDOWN(H95/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>25</v>
       </c>
       <c r="J95" s="15">
@@ -12072,14 +12072,14 @@
         <v>131</v>
       </c>
       <c r="G96" s="20">
-        <f>F96/10/C96</f>
+        <f t="shared" si="4"/>
         <v>0.15975609756097561</v>
       </c>
       <c r="H96" s="18">
         <v>24609</v>
       </c>
       <c r="I96" s="13">
-        <f>ROUNDDOWN(H96/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="J96" s="15">
@@ -12144,14 +12144,14 @@
         <v>179</v>
       </c>
       <c r="G97" s="20">
-        <f>F97/10/C97</f>
+        <f t="shared" si="4"/>
         <v>0.17899999999999999</v>
       </c>
       <c r="H97" s="18">
         <v>35156</v>
       </c>
       <c r="I97" s="13">
-        <f>ROUNDDOWN(H97/1171,0)</f>
+        <f t="shared" si="5"/>
         <v>30</v>
       </c>
       <c r="J97" s="15">
@@ -12216,14 +12216,14 @@
         <v>238</v>
       </c>
       <c r="G98" s="20">
-        <f>F98/10/C98</f>
+        <f t="shared" ref="G98:G129" si="6">F98/10/C98</f>
         <v>0.22884615384615387</v>
       </c>
       <c r="H98" s="18">
         <v>166406</v>
       </c>
       <c r="I98" s="13">
-        <f>ROUNDDOWN(H98/1171,0)</f>
+        <f t="shared" ref="I98:I129" si="7">ROUNDDOWN(H98/1171,0)</f>
         <v>142</v>
       </c>
       <c r="J98" s="15">
@@ -12288,14 +12288,14 @@
         <v>228</v>
       </c>
       <c r="G99" s="20">
-        <f>F99/10/C99</f>
+        <f t="shared" si="6"/>
         <v>0.23265306122448981</v>
       </c>
       <c r="H99" s="18">
         <v>203906</v>
       </c>
       <c r="I99" s="13">
-        <f>ROUNDDOWN(H99/1171,0)</f>
+        <f t="shared" si="7"/>
         <v>174</v>
       </c>
       <c r="J99" s="15">
@@ -12360,14 +12360,14 @@
         <v>119</v>
       </c>
       <c r="G100" s="23">
-        <f>F100/10/C100</f>
+        <f t="shared" si="6"/>
         <v>8.380281690140845E-2</v>
       </c>
       <c r="H100" s="24">
         <v>37500</v>
       </c>
       <c r="I100" s="21">
-        <f>ROUNDDOWN(H100/1171,0)</f>
+        <f t="shared" si="7"/>
         <v>32</v>
       </c>
       <c r="J100" s="22">
@@ -12425,14 +12425,14 @@
         <v>172</v>
       </c>
       <c r="G101" s="23">
-        <f>F101/10/C101</f>
+        <f t="shared" si="6"/>
         <v>0.11096774193548387</v>
       </c>
       <c r="H101" s="24">
         <v>42187</v>
       </c>
       <c r="I101" s="21">
-        <f>ROUNDDOWN(H101/1171,0)</f>
+        <f t="shared" si="7"/>
         <v>36</v>
       </c>
       <c r="J101" s="22">
@@ -12529,19 +12529,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N99 P102:Q1048576">
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="17" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12576,19 +12576,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N100">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="9" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12623,19 +12623,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N101">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12650,8 +12650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7172A816-79DD-4357-AD25-A7860CFF91DA}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M11" activeCellId="1" sqref="M14 M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
empty sheets for all wagons
</commit_message>
<xml_diff>
--- a/Worksheet.xlsx
+++ b/Worksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Documents\GRFStuff\UK Finescale Set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBBFCB0-9372-453D-8CDC-6E9105EF26BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832CC4FB-C160-4DC8-844C-87A2A3B1A17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{857BF7F3-4843-4495-BC2D-6D08C3451E58}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{857BF7F3-4843-4495-BC2D-6D08C3451E58}"/>
   </bookViews>
   <sheets>
     <sheet name="Name Stuff" sheetId="4" r:id="rId1"/>
@@ -2201,118 +2201,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="59">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2666,6 +2554,13 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3230,6 +3125,111 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3244,42 +3244,42 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7575EDDE-3AAA-4483-ACE3-DCAE8EA3E8E7}" name="Table2" displayName="Table2" ref="A1:T105" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7575EDDE-3AAA-4483-ACE3-DCAE8EA3E8E7}" name="Table2" displayName="Table2" ref="A1:T105" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:T105" xr:uid="{36D57E6B-8B33-4ACF-A7F0-0856AF37967D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T101">
     <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{68CBBF4D-117B-46E6-B7A4-54509CD6E6FB}" name="ID" dataDxfId="56"/>
-    <tableColumn id="19" xr3:uid="{03AC1107-CE99-4984-A642-BF90BC17A239}" name="UKRS Name" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{BF20BF4A-0C5E-449A-ACE9-902DD6F25C69}" name="Weight" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{6F02F023-E63F-47BD-8453-9990FFD54AA5}" name="Speed" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{93D71C14-746F-4DF8-A137-B414A2B01F0B}" name="Power" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{4B59892B-E1F2-4F5C-BD85-8447BA247813}" name="TE" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{AC10C65A-66CC-4985-B3F7-B0FB085872AF}" name="TE Coeff" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{68CBBF4D-117B-46E6-B7A4-54509CD6E6FB}" name="ID" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{03AC1107-CE99-4984-A642-BF90BC17A239}" name="UKRS Name" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{BF20BF4A-0C5E-449A-ACE9-902DD6F25C69}" name="Weight" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{6F02F023-E63F-47BD-8453-9990FFD54AA5}" name="Speed" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{93D71C14-746F-4DF8-A137-B414A2B01F0B}" name="Power" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{4B59892B-E1F2-4F5C-BD85-8447BA247813}" name="TE" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{AC10C65A-66CC-4985-B3F7-B0FB085872AF}" name="TE Coeff" dataDxfId="35">
       <calculatedColumnFormula>F2/10/C2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{C806CAA6-3838-4674-880C-06C79D31398A}" name="Air Drag" dataDxfId="49"/>
-    <tableColumn id="23" xr3:uid="{135FB07C-1FE9-48C6-A372-142B86E05EA8}" name="Air Drag Coef." dataDxfId="48">
+    <tableColumn id="17" xr3:uid="{C806CAA6-3838-4674-880C-06C79D31398A}" name="Air Drag" dataDxfId="34"/>
+    <tableColumn id="23" xr3:uid="{135FB07C-1FE9-48C6-A372-142B86E05EA8}" name="Air Drag Coef." dataDxfId="33">
       <calculatedColumnFormula>ROUND((Table2[[#This Row],[Air Drag]]+0.3504)/293.4,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{7CCBBFAF-1597-42B4-A0E0-8848B36F3A85}" name="Cost" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{A935D94E-3872-4036-A743-42E97F0A5706}" name="Cost Factor" dataDxfId="46">
+    <tableColumn id="8" xr3:uid="{7CCBBFAF-1597-42B4-A0E0-8848B36F3A85}" name="Cost" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{A935D94E-3872-4036-A743-42E97F0A5706}" name="Cost Factor" dataDxfId="31">
       <calculatedColumnFormula>ROUNDDOWN(J2/1171,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{025F4854-003D-4C1D-86DE-3CE439FE9C7E}" name="RC Factor?" dataDxfId="45">
+    <tableColumn id="11" xr3:uid="{025F4854-003D-4C1D-86DE-3CE439FE9C7E}" name="RC Factor?" dataDxfId="30">
       <calculatedColumnFormula>Table2[[#This Row],[RunCost]]/(23400/255)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{5BCDCD29-35DE-42FD-B065-4D759BF7D38E}" name="New RC" dataDxfId="44">
+    <tableColumn id="14" xr3:uid="{5BCDCD29-35DE-42FD-B065-4D759BF7D38E}" name="New RC" dataDxfId="29">
       <calculatedColumnFormula array="1">_xlfn.SWITCH(Table2[[#This Row],[Propulsion]],"S",Table2[[#This Row],[Cost Factor]]*(2090/255),"D",Table2[[#This Row],[Cost Factor]]*(1942/255),"E",Table2[[#This Row],[Cost Factor]]*(1792/255),"M",Table2[[#This Row],[Cost Factor]]*(1792/255),3,Table2[[#This Row],[Cost Factor]]*(1792/255))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{4EF97444-7DF2-4C1C-9399-2AF176D2421D}" name="RunCost" dataDxfId="43"/>
-    <tableColumn id="12" xr3:uid="{1BC97C8C-0238-41D7-8180-11A9FE8439B0}" name="Intro Year" dataDxfId="42"/>
-    <tableColumn id="13" xr3:uid="{5B6AB601-40E1-4161-8BD3-27417D3EF971}" name="Propulsion" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{3DD9EBC7-6915-4B09-94B8-EB93AD555BB9}" name="Length" dataDxfId="40"/>
-    <tableColumn id="16" xr3:uid="{6FAB79C9-0044-4515-B975-0FECD4FE0705}" name="Whistle" dataDxfId="39"/>
-    <tableColumn id="2" xr3:uid="{7544EFBE-4B04-489D-B161-77017965D88F}" name="Name" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{AB5CB6B3-E247-433B-9AAE-1FAD1BCAC333}" name="FullName" dataDxfId="37">
+    <tableColumn id="10" xr3:uid="{4EF97444-7DF2-4C1C-9399-2AF176D2421D}" name="RunCost" dataDxfId="28"/>
+    <tableColumn id="12" xr3:uid="{1BC97C8C-0238-41D7-8180-11A9FE8439B0}" name="Intro Year" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{5B6AB601-40E1-4161-8BD3-27417D3EF971}" name="Propulsion" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{3DD9EBC7-6915-4B09-94B8-EB93AD555BB9}" name="Length" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{6FAB79C9-0044-4515-B975-0FECD4FE0705}" name="Whistle" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{7544EFBE-4B04-489D-B161-77017965D88F}" name="Name" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{AB5CB6B3-E247-433B-9AAE-1FAD1BCAC333}" name="FullName" dataDxfId="22">
       <calculatedColumnFormula>CONCATENATE(Table2[[#This Row],[Name]]," - (",Table2[[#This Row],[UKRS Name]],")")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3288,40 +3288,40 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86C7D809-E0DA-4679-B4A9-491D10C625C4}" name="Table1" displayName="Table1" ref="A1:S100" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86C7D809-E0DA-4679-B4A9-491D10C625C4}" name="Table1" displayName="Table1" ref="A1:S100" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:S100" xr:uid="{86C7D809-E0DA-4679-B4A9-491D10C625C4}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{F0988B62-1E4B-4DA4-AF85-98CF7A0BB62C}" name="ID" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{6C3DAFD2-B5B6-4947-BC53-A9C9458F0725}" name="Name" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{ED9D427A-4B36-45C7-A02F-8BD0DD77B5E9}" name="Weight" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{9548E84D-C4FE-46B2-9350-6028631F9F44}" name="Speed" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{20748489-081E-419D-AC6B-372FE5768A07}" name="Cost" dataDxfId="30"/>
-    <tableColumn id="15" xr3:uid="{6CEDAC5A-5CFC-4919-802C-D4A941BB54CE}" name="New Cost" dataDxfId="29">
+    <tableColumn id="1" xr3:uid="{F0988B62-1E4B-4DA4-AF85-98CF7A0BB62C}" name="ID" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{6C3DAFD2-B5B6-4947-BC53-A9C9458F0725}" name="Name" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{ED9D427A-4B36-45C7-A02F-8BD0DD77B5E9}" name="Weight" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{9548E84D-C4FE-46B2-9350-6028631F9F44}" name="Speed" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{20748489-081E-419D-AC6B-372FE5768A07}" name="Cost" dataDxfId="14"/>
+    <tableColumn id="15" xr3:uid="{6CEDAC5A-5CFC-4919-802C-D4A941BB54CE}" name="New Cost" dataDxfId="13">
       <calculatedColumnFormula>ROUNDDOWN((1494/255)*Table1[[#This Row],[Cost Factor]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{EF424F8F-7FA6-4793-BF3A-60DD9EEB7163}" name="Cost Factor" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{EF424F8F-7FA6-4793-BF3A-60DD9EEB7163}" name="Cost Factor" dataDxfId="12">
       <calculatedColumnFormula>VLOOKUP(Table1[[#This Row],[Cost]],'Wagon Costs'!D:E,2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F73465CE-43D8-4293-B6BF-5D5365C10B22}" name="RC Factor?" dataDxfId="27">
+    <tableColumn id="7" xr3:uid="{F73465CE-43D8-4293-B6BF-5D5365C10B22}" name="RC Factor?" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[RunCost]]/(124/255)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{9B59C6C3-FB3F-4980-9AB3-5A1CEEC459C2}" name="New RC" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{9B59C6C3-FB3F-4980-9AB3-5A1CEEC459C2}" name="New RC" dataDxfId="10">
       <calculatedColumnFormula>IF(X2=1,Table1[[#This Row],[RC Factor?]]*(1792/255),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{6DF48C41-8E9F-4153-A1C2-66E9BC9790CA}" name="RunCost" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{B2A0025E-CFA5-46F8-98DD-509D6B8E2167}" name="Intro Year" dataDxfId="24"/>
-    <tableColumn id="11" xr3:uid="{2E946355-C8E5-4B63-BC77-D6B0FE9522B9}" name="Length" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{0BDF56F8-A331-4829-8791-E172F6D37265}" name="Capacity (D)" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{32219701-A423-4708-8B46-93D5CBAB6AD2}" name="Capacity (2)" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{6DF48C41-8E9F-4153-A1C2-66E9BC9790CA}" name="RunCost" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{B2A0025E-CFA5-46F8-98DD-509D6B8E2167}" name="Intro Year" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{2E946355-C8E5-4B63-BC77-D6B0FE9522B9}" name="Length" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{0BDF56F8-A331-4829-8791-E172F6D37265}" name="Capacity (D)" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{32219701-A423-4708-8B46-93D5CBAB6AD2}" name="Capacity (2)" dataDxfId="5">
       <calculatedColumnFormula>Table1[[#This Row],[Capacity (D)]]*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{82FC54E3-BC6E-4FAD-9DB7-25D6FC06B77F}" name="Capacity (4)" dataDxfId="20">
+    <tableColumn id="19" xr3:uid="{82FC54E3-BC6E-4FAD-9DB7-25D6FC06B77F}" name="Capacity (4)" dataDxfId="4">
       <calculatedColumnFormula>Table1[[#This Row],[Capacity (D)]]*4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{3F4C0448-F5B2-49FF-A4B0-B6C47E30AF5C}" name="Capacity (R)" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{ED1CEE75-E7B9-4CB0-9E2A-4140191C4EE4}" name="Capacity (T)" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{692F26B5-5EE4-424C-A39C-048687D2AD44}" name="Carries" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{A96C7EAA-24E2-4227-9C9D-044DD168DC44}" name="Alt Name" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{3F4C0448-F5B2-49FF-A4B0-B6C47E30AF5C}" name="Capacity (R)" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{ED1CEE75-E7B9-4CB0-9E2A-4140191C4EE4}" name="Capacity (T)" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{692F26B5-5EE4-424C-A39C-048687D2AD44}" name="Carries" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{A96C7EAA-24E2-4227-9C9D-044DD168DC44}" name="Alt Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14878,9 +14878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D8F614-8F67-461D-B4C9-7B9798EA7994}">
   <dimension ref="A1:AD105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23071,19 +23071,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P99 R102:S1048576">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="17" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="18" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="19" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="20" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="21" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23118,19 +23118,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P100">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="9" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="10" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="12" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="13" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23165,24 +23165,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P101">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="1" operator="equal">
       <formula>"M"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="equal">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="5" operator="equal">
       <formula>"S"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q33" twoDigitTextYear="1"/>
+  </ignoredErrors>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -23193,9 +23196,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85BF7ED-5695-4CE1-BF5A-80E789BE5EBA}">
   <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23710,7 +23713,9 @@
       <c r="J8" s="42">
         <v>74</v>
       </c>
-      <c r="K8" s="37"/>
+      <c r="K8" s="37">
+        <v>1948</v>
+      </c>
       <c r="L8" s="37">
         <v>8</v>
       </c>
@@ -23773,7 +23778,9 @@
       <c r="J9" s="42">
         <v>74</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="37">
+        <v>1969</v>
+      </c>
       <c r="L9" s="37">
         <v>8</v>
       </c>
@@ -23836,7 +23843,9 @@
       <c r="J10" s="42">
         <v>74</v>
       </c>
-      <c r="K10" s="37"/>
+      <c r="K10" s="37">
+        <v>1985</v>
+      </c>
       <c r="L10" s="37">
         <v>8</v>
       </c>
@@ -23964,7 +23973,9 @@
       <c r="J12" s="42">
         <v>74</v>
       </c>
-      <c r="K12" s="37"/>
+      <c r="K12" s="37">
+        <v>1985</v>
+      </c>
       <c r="L12" s="37">
         <v>8</v>
       </c>
@@ -24027,7 +24038,9 @@
       <c r="J13" s="42">
         <v>74</v>
       </c>
-      <c r="K13" s="37"/>
+      <c r="K13" s="37">
+        <v>2000</v>
+      </c>
       <c r="L13" s="37">
         <v>8</v>
       </c>
@@ -24415,7 +24428,9 @@
       <c r="J19" s="42">
         <v>34</v>
       </c>
-      <c r="K19" s="37"/>
+      <c r="K19" s="37">
+        <v>1969</v>
+      </c>
       <c r="L19" s="37">
         <v>7</v>
       </c>
@@ -24478,7 +24493,9 @@
       <c r="J20" s="42">
         <v>34</v>
       </c>
-      <c r="K20" s="37"/>
+      <c r="K20" s="37">
+        <v>1985</v>
+      </c>
       <c r="L20" s="37">
         <v>7</v>
       </c>
@@ -28521,7 +28538,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I100">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="colorScale" priority="5">

</xml_diff>